<commit_message>
feat: Add multiple functionalities
1. exception handling in all functions
2. logging in proper manner
3. selecting elements in proper manner
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Product Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,6 +420,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="168" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -461,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>
@@ -483,7 +489,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>
@@ -505,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>
@@ -527,7 +533,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>
@@ -549,7 +555,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>
@@ -571,7 +577,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-06-25 18:59:30</t>
+          <t>2025-06-26 14:16:26</t>
         </is>
       </c>
     </row>

</xml_diff>